<commit_message>
Add model 3 analysis and update report
</commit_message>
<xml_diff>
--- a/data/raw-data/exampledata2.xlsx
+++ b/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12E657BD-D407-4C3C-8C28-7B852E62B080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{12E657BD-D407-4C3C-8C28-7B852E62B080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52054110-3FF2-42E5-816C-76B93D095B37}"/>
   <bookViews>
-    <workbookView xWindow="7425" yWindow="0" windowWidth="13170" windowHeight="10905" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8145" yWindow="1635" windowWidth="10725" windowHeight="9030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,15 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>Height</t>
   </si>
   <si>
     <t>Weight</t>
-  </si>
-  <si>
-    <t>sixty</t>
   </si>
   <si>
     <t>M</t>
@@ -427,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,13 +438,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -458,13 +455,13 @@
         <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -475,30 +472,30 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
+      <c r="A4">
+        <v>75</v>
       </c>
       <c r="B4">
         <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>7.5</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -509,13 +506,13 @@
         <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -526,13 +523,13 @@
         <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -543,13 +540,13 @@
         <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -560,13 +557,13 @@
         <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -577,13 +574,13 @@
         <v>110</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -594,13 +591,13 @@
         <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10">
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -611,13 +608,13 @@
         <v>7000</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -625,13 +622,13 @@
         <v>165</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12">
         <v>6.5</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -642,13 +639,13 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -659,13 +656,13 @@
         <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -676,13 +673,13 @@
         <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -694,7 +691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -707,13 +704,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -721,10 +718,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -732,43 +729,43 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
         <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>